<commit_message>
Published state of ETDataset on 8 September 2014.
</commit_message>
<xml_diff>
--- a/source_analyses/eu/2012/2_power_and_heat_plant/hydro_source_analysis.xlsx
+++ b/source_analyses/eu/2012/2_power_and_heat_plant/hydro_source_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2600" yWindow="860" windowWidth="38400" windowHeight="21800" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro" sheetId="1" r:id="rId1"/>
@@ -79,10 +79,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -226,59 +234,81 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="36">
+  <cellStyles count="57">
     <cellStyle name="E_InputWhite" xfId="4"/>
     <cellStyle name="E_SecTitle1" xfId="1"/>
     <cellStyle name="E_SecTitle2" xfId="2"/>
@@ -299,6 +329,16 @@
     <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
@@ -314,7 +354,18 @@
     <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="36" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -646,7 +697,7 @@
   <dimension ref="B2:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -724,19 +775,19 @@
         <v>2</v>
       </c>
       <c r="C13" s="6">
-        <v>3548.6364102564103</v>
+        <v>3588</v>
       </c>
       <c r="D13" s="4">
         <f>C13*$C$3*0.0036</f>
-        <v>31937.727692307693</v>
-      </c>
-      <c r="E13" s="2">
+        <v>32292</v>
+      </c>
+      <c r="E13" s="8">
         <f>D13/SUM(D13:D14)</f>
-        <v>0.62867404600382615</v>
+        <v>0.21645816897168266</v>
       </c>
       <c r="F13" s="4">
         <f>$C$3*C10/SUM(D13:D14)</f>
-        <v>3754.7148229937552</v>
+        <v>1278.5993403527991</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="16" thickBot="1">
@@ -744,19 +795,19 @@
         <v>6</v>
       </c>
       <c r="C14" s="6">
-        <v>1310</v>
+        <v>8117.4693679999982</v>
       </c>
       <c r="D14" s="4">
         <f>C14*$C$4*0.0036</f>
-        <v>18864</v>
-      </c>
-      <c r="E14" s="2">
+        <v>116891.55889919997</v>
+      </c>
+      <c r="E14" s="8">
         <f>D14/SUM(D13:D14)</f>
-        <v>0.37132595399617391</v>
+        <v>0.78354183102831731</v>
       </c>
       <c r="F14" s="4">
         <f>$C$4*C10/SUM(D13:D14)</f>
-        <v>6007.5437167900081</v>
+        <v>2045.7589445644787</v>
       </c>
     </row>
     <row r="17" spans="2:6" ht="16" thickBot="1">

</xml_diff>

<commit_message>
Published state of ETDataset on 3 August 2018
</commit_message>
<xml_diff>
--- a/source_analyses/eu/2012/2_power_and_heat_plant/hydro_source_analysis.xlsx
+++ b/source_analyses/eu/2012/2_power_and_heat_plant/hydro_source_analysis.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexander/Git/etdataset/source_analyses/eu/2012/2_power_and_heat_plant/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ADA861-BE64-584F-8FAD-2111065550FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydro" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -78,12 +84,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -309,11 +315,11 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="57">
-    <cellStyle name="E_InputWhite" xfId="4"/>
-    <cellStyle name="E_SecTitle1" xfId="1"/>
-    <cellStyle name="E_SecTitle2" xfId="2"/>
-    <cellStyle name="E_Source" xfId="5"/>
-    <cellStyle name="E_TableHeader0" xfId="3"/>
+    <cellStyle name="E_InputWhite" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="E_SecTitle1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="E_SecTitle2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="E_Source" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="E_TableHeader0" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
@@ -369,6 +375,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -693,14 +707,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
@@ -740,7 +754,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="16" thickBot="1">
+    <row r="9" spans="2:6" ht="17" thickBot="1">
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
@@ -748,15 +762,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="16" thickBot="1">
+    <row r="10" spans="2:6" ht="17" thickBot="1">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="6">
-        <v>76298.400000000009</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="16" thickBot="1">
+        <v>68317</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="17" thickBot="1">
       <c r="C12" s="7" t="s">
         <v>8</v>
       </c>
@@ -770,47 +784,47 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:6" ht="16" thickBot="1">
+    <row r="13" spans="2:6" ht="17" thickBot="1">
       <c r="B13" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="6">
-        <v>3588</v>
+        <v>3749.0329999999972</v>
       </c>
       <c r="D13" s="4">
         <f>C13*$C$3*0.0036</f>
-        <v>32292</v>
+        <v>33741.29699999997</v>
       </c>
       <c r="E13" s="8">
         <f>D13/SUM(D13:D14)</f>
-        <v>0.21645816897168266</v>
+        <v>0.90394058204195216</v>
       </c>
       <c r="F13" s="4">
         <f>$C$3*C10/SUM(D13:D14)</f>
-        <v>1278.5993403527991</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="16" thickBot="1">
+        <v>4575.5879466755605</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="17" thickBot="1">
       <c r="B14" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="6">
-        <v>8117.4693679999982</v>
+        <v>249</v>
       </c>
       <c r="D14" s="4">
         <f>C14*$C$4*0.0036</f>
-        <v>116891.55889919997</v>
+        <v>3585.6</v>
       </c>
       <c r="E14" s="8">
         <f>D14/SUM(D13:D14)</f>
-        <v>0.78354183102831731</v>
+        <v>9.6059417958047871E-2</v>
       </c>
       <c r="F14" s="4">
         <f>$C$4*C10/SUM(D13:D14)</f>
-        <v>2045.7589445644787</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="16" thickBot="1">
+        <v>7320.9407146808971</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="17" thickBot="1">
       <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
@@ -818,7 +832,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="16" thickBot="1">
+    <row r="18" spans="2:6" ht="17" thickBot="1">
       <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
@@ -826,7 +840,7 @@
         <v>73962</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="16" thickBot="1">
+    <row r="20" spans="2:6" ht="17" thickBot="1">
       <c r="C20" s="7" t="s">
         <v>8</v>
       </c>
@@ -840,7 +854,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="16" thickBot="1">
+    <row r="21" spans="2:6" ht="17" thickBot="1">
       <c r="B21" t="s">
         <v>2</v>
       </c>
@@ -860,7 +874,7 @@
         <v>830.51710756095986</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="16" thickBot="1">
+    <row r="22" spans="2:6" ht="17" thickBot="1">
       <c r="B22" t="s">
         <v>6</v>
       </c>
@@ -880,7 +894,7 @@
         <v>1328.8273720975358</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="16" thickBot="1">
+    <row r="25" spans="2:6" ht="17" thickBot="1">
       <c r="B25" s="3" t="s">
         <v>5</v>
       </c>
@@ -888,7 +902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="16" thickBot="1">
+    <row r="26" spans="2:6" ht="17" thickBot="1">
       <c r="B26" s="3" t="s">
         <v>7</v>
       </c>
@@ -896,7 +910,7 @@
         <v>211381.19999999998</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="16" thickBot="1">
+    <row r="28" spans="2:6" ht="17" thickBot="1">
       <c r="C28" s="7" t="s">
         <v>8</v>
       </c>
@@ -910,7 +924,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="16" thickBot="1">
+    <row r="29" spans="2:6" ht="17" thickBot="1">
       <c r="B29" t="s">
         <v>2</v>
       </c>
@@ -930,7 +944,7 @@
         <v>1755.8386411889594</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="16" thickBot="1">
+    <row r="30" spans="2:6" ht="17" thickBot="1">
       <c r="B30" t="s">
         <v>6</v>
       </c>
@@ -950,7 +964,7 @@
         <v>2809.3418259023351</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="16" thickBot="1">
+    <row r="33" spans="2:6" ht="17" thickBot="1">
       <c r="B33" s="3" t="s">
         <v>5</v>
       </c>
@@ -958,7 +972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="16" thickBot="1">
+    <row r="34" spans="2:6" ht="17" thickBot="1">
       <c r="B34" s="3" t="s">
         <v>7</v>
       </c>
@@ -966,7 +980,7 @@
         <v>19025.999999999996</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="16" thickBot="1">
+    <row r="36" spans="2:6" ht="17" thickBot="1">
       <c r="C36" s="7" t="s">
         <v>8</v>
       </c>
@@ -980,7 +994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="16" thickBot="1">
+    <row r="37" spans="2:6" ht="17" thickBot="1">
       <c r="B37" t="s">
         <v>2</v>
       </c>
@@ -1000,7 +1014,7 @@
         <v>2022.5794106391118</v>
       </c>
     </row>
-    <row r="38" spans="2:6" ht="16" thickBot="1">
+    <row r="38" spans="2:6" ht="17" thickBot="1">
       <c r="B38" t="s">
         <v>6</v>
       </c>
@@ -1020,7 +1034,7 @@
         <v>3236.1270570225788</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="16" thickBot="1">
+    <row r="41" spans="2:6" ht="17" thickBot="1">
       <c r="B41" s="3" t="s">
         <v>5</v>
       </c>
@@ -1028,7 +1042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="16" thickBot="1">
+    <row r="42" spans="2:6" ht="17" thickBot="1">
       <c r="B42" s="3" t="s">
         <v>7</v>
       </c>
@@ -1036,7 +1050,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="44" spans="2:6" ht="16" thickBot="1">
+    <row r="44" spans="2:6" ht="17" thickBot="1">
       <c r="C44" s="7" t="s">
         <v>8</v>
       </c>
@@ -1050,7 +1064,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="16" thickBot="1">
+    <row r="45" spans="2:6" ht="17" thickBot="1">
       <c r="B45" t="s">
         <v>2</v>
       </c>
@@ -1070,7 +1084,7 @@
         <v>2515.0150150150148</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="16" thickBot="1">
+    <row r="46" spans="2:6" ht="17" thickBot="1">
       <c r="B46" t="s">
         <v>6</v>
       </c>
@@ -1090,7 +1104,7 @@
         <v>4024.0240240240241</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="16" thickBot="1">
+    <row r="49" spans="2:6" ht="17" thickBot="1">
       <c r="B49" s="3" t="s">
         <v>5</v>
       </c>
@@ -1098,7 +1112,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="16" thickBot="1">
+    <row r="50" spans="2:6" ht="17" thickBot="1">
       <c r="B50" s="3" t="s">
         <v>7</v>
       </c>
@@ -1106,7 +1120,7 @@
         <v>7333</v>
       </c>
     </row>
-    <row r="52" spans="2:6" ht="16" thickBot="1">
+    <row r="52" spans="2:6" ht="17" thickBot="1">
       <c r="C52" s="7" t="s">
         <v>8</v>
       </c>
@@ -1120,7 +1134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="2:6" ht="16" thickBot="1">
+    <row r="53" spans="2:6" ht="17" thickBot="1">
       <c r="B53" t="s">
         <v>2</v>
       </c>
@@ -1140,7 +1154,7 @@
         <v>1383.9818212015523</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="16" thickBot="1">
+    <row r="54" spans="2:6" ht="17" thickBot="1">
       <c r="B54" t="s">
         <v>6</v>
       </c>

</xml_diff>